<commit_message>
proxt chrome arguments test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B74624D-7573-2146-9A0B-39D60ECB415F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1E1ECC-119E-234C-98A0-DA5142BB6139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>PROXY</t>
+  </si>
+  <si>
+    <t>51.159.207.156:3128</t>
+  </si>
+  <si>
+    <t>200.105.215.18:33630</t>
+  </si>
+  <si>
+    <t>20.54.56.26:8080</t>
+  </si>
+  <si>
+    <t>145.40.77.207:3128</t>
+  </si>
+  <si>
+    <t>182.253.172.20:8080</t>
+  </si>
+  <si>
+    <t>45.233.67.230:999</t>
+  </si>
+  <si>
+    <t>51.159.162.151:80</t>
+  </si>
+  <si>
+    <t>190.121.207.58:999</t>
+  </si>
+  <si>
+    <t>181.129.49.214:999</t>
   </si>
 </sst>
 </file>
@@ -388,7 +415,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -414,60 +441,90 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>

</xml_diff>

<commit_message>
Before each method, the driver works with a different ip address
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="28">
   <si>
     <t>PROXY</t>
   </si>
@@ -53,12 +53,67 @@
   </si>
   <si>
     <t>181.129.49.214:999</t>
+  </si>
+  <si>
+    <t>142.93.2.136:8080</t>
+  </si>
+  <si>
+    <t>35.187.4.12:8888</t>
+  </si>
+  <si>
+    <t>35.233.30.201:3128</t>
+  </si>
+  <si>
+    <t>185.157.1.249:3128</t>
+  </si>
+  <si>
+    <t>157.100.12.138:999</t>
+  </si>
+  <si>
+    <t>118.42.15.57:4003</t>
+  </si>
+  <si>
+    <t>43.158.209.151:8888</t>
+  </si>
+  <si>
+    <t>49.0.2.242:8090</t>
+  </si>
+  <si>
+    <t>157.230.217.232:8080</t>
+  </si>
+  <si>
+    <t>116.58.254.126:8080</t>
+  </si>
+  <si>
+    <t>137.184.103.147:8080</t>
+  </si>
+  <si>
+    <t>45.169.162.1:3128</t>
+  </si>
+  <si>
+    <t>116.107.57.229:4047</t>
+  </si>
+  <si>
+    <t>83.229.73.175:80</t>
+  </si>
+  <si>
+    <t>177.12.238.1:3128</t>
+  </si>
+  <si>
+    <t>89.107.197.165:3128</t>
+  </si>
+  <si>
+    <t>191.97.19.18:999</t>
+  </si>
+  <si>
+    <t>177.12.238.100:3128</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,12 +475,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="45.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="25.5"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="19.33203125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="28.5"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.5"/>
+    <col min="6" max="10" customWidth="true" width="20.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -442,7 +497,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -460,7 +515,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -469,7 +524,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -478,7 +533,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -487,7 +542,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -496,7 +551,7 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -505,7 +560,7 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -514,7 +569,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -523,7 +578,7 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>

</xml_diff>